<commit_message>
Added Excel template export support formula
</commit_message>
<xml_diff>
--- a/src/Magicodes.ExporterAndImporter.Tests/TestFiles/ExportTemplates/2020年春季教材订购明细样表.xlsx
+++ b/src/Magicodes.ExporterAndImporter.Tests/TestFiles/ExportTemplates/2020年春季教材订购明细样表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Person\HueiFeng\Magicodes.IE\src\Magicodes.ExporterAndImporter.Tests\TestFiles\ExportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5EC2C2-E89A-4D6C-B31D-9138231C37F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E116DC9D-2203-41E5-862B-BFF93EB91C9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>序号</t>
   </si>
@@ -111,7 +111,7 @@
   </si>
   <si>
     <r>
-      <t>{{Formula::SUM?number=G5</t>
+      <t>{{Formula::SUM?params=G4:G6&amp;G4</t>
     </r>
     <r>
       <rPr>
@@ -123,6 +123,14 @@
       </rPr>
       <t>}}</t>
     </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>平均：</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Formula::AVERAGE?params=G4:G6}}</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -323,7 +331,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -379,6 +387,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -660,7 +677,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -784,17 +801,28 @@
       </c>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H10" s="20"/>
+    </row>
     <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
Add test issue #142
</commit_message>
<xml_diff>
--- a/src/Magicodes.ExporterAndImporter.Tests/TestFiles/ExportTemplates/2020年春季教材订购明细样表.xlsx
+++ b/src/Magicodes.ExporterAndImporter.Tests/TestFiles/ExportTemplates/2020年春季教材订购明细样表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Person\HueiFeng\Magicodes.IE\src\Magicodes.ExporterAndImporter.Tests\TestFiles\ExportTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\HueiFeng\Magicodes.IE\src\Magicodes.ExporterAndImporter.Tests\TestFiles\ExportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FC119E-5342-4E1F-B310-3F6741925B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B582CB4C-9336-494D-BF82-85C56F7E3B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,10 +102,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>{{Image::Cover?Alt=无封面}}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>合计：</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -118,7 +114,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>}}</t>
@@ -131,6 +126,10 @@
   </si>
   <si>
     <t>{{Formula::AVERAGE?params=G4:G6}}</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Image::Cover?w=60&amp;h=60&amp;Alt=无封面}}</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -141,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,7 +151,6 @@
     <font>
       <sz val="11"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -160,7 +158,6 @@
       <sz val="18"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -168,7 +165,6 @@
       <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -177,7 +173,6 @@
       <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -185,7 +180,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -193,20 +187,17 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -229,6 +220,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -331,7 +329,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -369,6 +367,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -677,47 +681,47 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.25" customWidth="1"/>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="3" max="3" width="27.125" customWidth="1"/>
-    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.75" customWidth="1"/>
-    <col min="9" max="9" width="37.125" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="27.08984375" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.08984375" customWidth="1"/>
+    <col min="9" max="9" width="37.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:9" ht="26.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:9" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="1:9" ht="37" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="19"/>
     </row>
-    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -746,7 +750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -768,54 +772,54 @@
       <c r="G4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>21</v>
+      <c r="H4" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="18" t="s">
+    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C8" t="s">
+    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="I8" s="21"/>
+    </row>
+    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="19"/>
+      <c r="H9" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="23"/>
     </row>
-    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="21"/>
-    </row>
-    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B1:I1"/>

</xml_diff>